<commit_message>
Leads on mu issue
</commit_message>
<xml_diff>
--- a/Examples/Studio/EllipsoidConstraints/optimize.xlsx
+++ b/Examples/Studio/EllipsoidConstraints/optimize.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="537">
   <si>
     <t>name</t>
   </si>
@@ -1403,211 +1403,79 @@
     <t>value_1</t>
   </si>
   <si>
-    <t>alignment_enabled</t>
+    <t>number_of_particles</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>initial_relative_weighting</t>
+  </si>
+  <si>
+    <t>0.010000</t>
+  </si>
+  <si>
+    <t>relative_weighting</t>
+  </si>
+  <si>
+    <t>1.000000</t>
+  </si>
+  <si>
+    <t>starting_regularization</t>
+  </si>
+  <si>
+    <t>ending_regularization</t>
+  </si>
+  <si>
+    <t>0.100000</t>
+  </si>
+  <si>
+    <t>iterations_per_split</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>optimization_iterations</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>use_geodesic_distance</t>
   </si>
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>alignment_method</t>
-  </si>
-  <si>
-    <t>Center</t>
-  </si>
-  <si>
-    <t>antialias</t>
-  </si>
-  <si>
-    <t>pad</t>
-  </si>
-  <si>
-    <t>pad_value</t>
+    <t>use_normals</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>normals_strength</t>
+  </si>
+  <si>
+    <t>10.000000</t>
+  </si>
+  <si>
+    <t>procrustes</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>procrustes_scaling</t>
+  </si>
+  <si>
+    <t>procrustes_rotation_translation</t>
+  </si>
+  <si>
+    <t>procrustes_interval</t>
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>fastmarching</t>
-  </si>
-  <si>
-    <t>blur</t>
-  </si>
-  <si>
-    <t>blur_sigma</t>
-  </si>
-  <si>
-    <t>2.000000</t>
-  </si>
-  <si>
-    <t>isolate</t>
-  </si>
-  <si>
-    <t>fill_holes</t>
-  </si>
-  <si>
-    <t>fill_mesh_holes</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>antialias_amount</t>
-  </si>
-  <si>
-    <t>groom_output_prefix</t>
-  </si>
-  <si>
-    <t>groomed1</t>
-  </si>
-  <si>
-    <t>convert_to_mesh</t>
-  </si>
-  <si>
-    <t>mesh_smooth</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_method</t>
-  </si>
-  <si>
-    <t>Laplacian</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_laplacian_iterations</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
-  </si>
-  <si>
-    <t>1.000000</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
-  </si>
-  <si>
-    <t>0.050000</t>
-  </si>
-  <si>
-    <t>crop</t>
-  </si>
-  <si>
-    <t>reflect</t>
-  </si>
-  <si>
-    <t>reflect_column</t>
-  </si>
-  <si>
-    <t>reflect_choice</t>
-  </si>
-  <si>
-    <t>reflect_axis</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>resample</t>
-  </si>
-  <si>
-    <t>isotropic</t>
-  </si>
-  <si>
-    <t>iso_spacing</t>
-  </si>
-  <si>
-    <t>spacing</t>
-  </si>
-  <si>
-    <t>1 1 1</t>
-  </si>
-  <si>
-    <t>remesh</t>
-  </si>
-  <si>
-    <t>remesh_percent_mode</t>
-  </si>
-  <si>
-    <t>remesh_percent</t>
-  </si>
-  <si>
-    <t>75.000000</t>
-  </si>
-  <si>
-    <t>remesh_num_vertices</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>remesh_gradation</t>
-  </si>
-  <si>
-    <t>groom_all_domains_the_same</t>
-  </si>
-  <si>
-    <t>number_of_particles</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>initial_relative_weighting</t>
-  </si>
-  <si>
-    <t>0.010000</t>
-  </si>
-  <si>
-    <t>relative_weighting</t>
-  </si>
-  <si>
-    <t>starting_regularization</t>
-  </si>
-  <si>
-    <t>ending_regularization</t>
-  </si>
-  <si>
-    <t>0.100000</t>
-  </si>
-  <si>
-    <t>iterations_per_split</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>optimization_iterations</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>use_geodesic_distance</t>
-  </si>
-  <si>
-    <t>use_normals</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>normals_strength</t>
-  </si>
-  <si>
-    <t>10.000000</t>
-  </si>
-  <si>
-    <t>procrustes</t>
-  </si>
-  <si>
-    <t>procrustes_scaling</t>
-  </si>
-  <si>
-    <t>procrustes_rotation_translation</t>
-  </si>
-  <si>
-    <t>procrustes_interval</t>
   </si>
   <si>
     <t>multiscale</t>
@@ -1674,7 +1542,7 @@
     <t>tool_state</t>
   </si>
   <si>
-    <t>groom</t>
+    <t>optimize</t>
   </si>
   <si>
     <t>version</t>
@@ -3780,7 +3648,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3792,286 +3660,6 @@
       </c>
       <c r="C1" t="s">
         <v>459</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>460</v>
-      </c>
-      <c r="C2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>462</v>
-      </c>
-      <c r="C3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>464</v>
-      </c>
-      <c r="C4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>465</v>
-      </c>
-      <c r="C5" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>466</v>
-      </c>
-      <c r="C6" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>468</v>
-      </c>
-      <c r="C7" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>469</v>
-      </c>
-      <c r="C8" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>470</v>
-      </c>
-      <c r="C9" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>472</v>
-      </c>
-      <c r="C10" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>473</v>
-      </c>
-      <c r="C11" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>474</v>
-      </c>
-      <c r="C12" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>476</v>
-      </c>
-      <c r="C13" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>477</v>
-      </c>
-      <c r="C14" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>479</v>
-      </c>
-      <c r="C15" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>480</v>
-      </c>
-      <c r="C16" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>481</v>
-      </c>
-      <c r="C17" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>483</v>
-      </c>
-      <c r="C18" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>484</v>
-      </c>
-      <c r="C19" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>486</v>
-      </c>
-      <c r="C20" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>487</v>
-      </c>
-      <c r="C21" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>489</v>
-      </c>
-      <c r="C22" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>490</v>
-      </c>
-      <c r="C23" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>491</v>
-      </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>492</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>493</v>
-      </c>
-      <c r="C26" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>495</v>
-      </c>
-      <c r="C27" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>496</v>
-      </c>
-      <c r="C28" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>497</v>
-      </c>
-      <c r="C29" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>498</v>
-      </c>
-      <c r="C30" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>500</v>
-      </c>
-      <c r="C31" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>501</v>
-      </c>
-      <c r="C32" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>502</v>
-      </c>
-      <c r="C33" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>504</v>
-      </c>
-      <c r="C34" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>506</v>
-      </c>
-      <c r="C35" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>507</v>
-      </c>
-      <c r="C36" t="s">
-        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -4093,162 +3681,162 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>508</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>510</v>
+        <v>462</v>
       </c>
       <c r="B3" t="s">
-        <v>511</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>512</v>
+        <v>464</v>
       </c>
       <c r="B4" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>513</v>
+        <v>466</v>
       </c>
       <c r="B5" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>514</v>
+        <v>467</v>
       </c>
       <c r="B6" t="s">
-        <v>515</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>516</v>
+        <v>469</v>
       </c>
       <c r="B7" t="s">
-        <v>517</v>
+        <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="B8" t="s">
-        <v>519</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>520</v>
+        <v>473</v>
       </c>
       <c r="B9" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>521</v>
+        <v>475</v>
       </c>
       <c r="B10" t="s">
-        <v>522</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>523</v>
+        <v>477</v>
       </c>
       <c r="B11" t="s">
-        <v>524</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>525</v>
+        <v>479</v>
       </c>
       <c r="B12" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>526</v>
+        <v>481</v>
       </c>
       <c r="B13" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>527</v>
+        <v>482</v>
       </c>
       <c r="B14" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>528</v>
+        <v>483</v>
       </c>
       <c r="B15" t="s">
-        <v>467</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>529</v>
+        <v>485</v>
       </c>
       <c r="B16" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>530</v>
+        <v>486</v>
       </c>
       <c r="B17" t="s">
-        <v>531</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>532</v>
+        <v>488</v>
       </c>
       <c r="B18" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>533</v>
+        <v>489</v>
       </c>
       <c r="B19" t="s">
-        <v>522</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>534</v>
+        <v>490</v>
       </c>
       <c r="B20" t="s">
-        <v>535</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>536</v>
+        <v>492</v>
       </c>
       <c r="B21" t="s">
-        <v>537</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -4270,50 +3858,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>538</v>
+        <v>494</v>
       </c>
       <c r="B2" t="s">
-        <v>539</v>
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>540</v>
+        <v>496</v>
       </c>
       <c r="B3" t="s">
-        <v>541</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>542</v>
+        <v>498</v>
       </c>
       <c r="B4" t="s">
-        <v>543</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>544</v>
+        <v>500</v>
       </c>
       <c r="B5" t="s">
-        <v>545</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>546</v>
+        <v>502</v>
       </c>
       <c r="B6" t="s">
-        <v>547</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>548</v>
+        <v>504</v>
       </c>
       <c r="B7" t="s">
-        <v>549</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -4335,10 +3923,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>550</v>
+        <v>506</v>
       </c>
       <c r="B2" t="s">
-        <v>551</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -4360,26 +3948,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>552</v>
+        <v>508</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>554</v>
+        <v>510</v>
       </c>
       <c r="B3" t="s">
-        <v>555</v>
+        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>556</v>
+        <v>512</v>
       </c>
       <c r="B4" t="s">
-        <v>557</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -4401,106 +3989,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>558</v>
+        <v>514</v>
       </c>
       <c r="B2" t="s">
-        <v>559</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>560</v>
+        <v>516</v>
       </c>
       <c r="B3" t="s">
-        <v>559</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>561</v>
+        <v>517</v>
       </c>
       <c r="B4" t="s">
-        <v>553</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>562</v>
+        <v>518</v>
       </c>
       <c r="B5" t="s">
-        <v>553</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>563</v>
+        <v>519</v>
       </c>
       <c r="B6" t="s">
-        <v>564</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>565</v>
+        <v>521</v>
       </c>
       <c r="B7" t="s">
-        <v>566</v>
+        <v>522</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>567</v>
+        <v>523</v>
       </c>
       <c r="B8" t="s">
-        <v>568</v>
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>569</v>
+        <v>525</v>
       </c>
       <c r="B9" t="s">
-        <v>570</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>571</v>
+        <v>527</v>
       </c>
       <c r="B10" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>572</v>
+        <v>528</v>
       </c>
       <c r="B11" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>573</v>
+        <v>529</v>
       </c>
       <c r="B12" t="s">
-        <v>551</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>574</v>
+        <v>530</v>
       </c>
       <c r="B13" t="s">
-        <v>575</v>
+        <v>531</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>576</v>
+        <v>532</v>
       </c>
       <c r="B14" t="s">
-        <v>570</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -4514,19 +4102,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>577</v>
+        <v>533</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>578</v>
+        <v>534</v>
       </c>
       <c r="D1" t="s">
-        <v>579</v>
+        <v>535</v>
       </c>
       <c r="E1" t="s">
-        <v>580</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted the constraints to where it was in October. This resembles the way constraints used to work more and overall works better once mu was removed. We should do further tests and possibly add Alan's improvements to this branch.
</commit_message>
<xml_diff>
--- a/Examples/Studio/EllipsoidConstraints/optimize.xlsx
+++ b/Examples/Studio/EllipsoidConstraints/optimize.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="582">
   <si>
     <t>name</t>
   </si>
@@ -1400,151 +1400,154 @@
     <t>value</t>
   </si>
   <si>
+    <t>alignment_enabled</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>alignment_method</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>antialias</t>
+  </si>
+  <si>
+    <t>pad</t>
+  </si>
+  <si>
+    <t>pad_value</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>fastmarching</t>
+  </si>
+  <si>
+    <t>blur</t>
+  </si>
+  <si>
+    <t>blur_sigma</t>
+  </si>
+  <si>
+    <t>2.000000</t>
+  </si>
+  <si>
+    <t>isolate</t>
+  </si>
+  <si>
+    <t>fill_holes</t>
+  </si>
+  <si>
+    <t>fill_mesh_holes</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>antialias_amount</t>
+  </si>
+  <si>
+    <t>groom_output_prefix</t>
+  </si>
+  <si>
+    <t>groomed1</t>
+  </si>
+  <si>
+    <t>convert_to_mesh</t>
+  </si>
+  <si>
+    <t>mesh_smooth</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_method</t>
+  </si>
+  <si>
+    <t>Laplacian</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
+  </si>
+  <si>
+    <t>1.000000</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
+  </si>
+  <si>
+    <t>0.050000</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>reflect</t>
+  </si>
+  <si>
+    <t>reflect_column</t>
+  </si>
+  <si>
+    <t>reflect_choice</t>
+  </si>
+  <si>
+    <t>reflect_axis</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>resample</t>
+  </si>
+  <si>
+    <t>isotropic</t>
+  </si>
+  <si>
+    <t>iso_spacing</t>
+  </si>
+  <si>
+    <t>spacing</t>
+  </si>
+  <si>
+    <t>1 1 1</t>
+  </si>
+  <si>
+    <t>remesh</t>
+  </si>
+  <si>
+    <t>remesh_percent_mode</t>
+  </si>
+  <si>
+    <t>remesh_percent</t>
+  </si>
+  <si>
+    <t>75.000000</t>
+  </si>
+  <si>
+    <t>remesh_num_vertices</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>remesh_gradation</t>
+  </si>
+  <si>
+    <t>skip_grooming</t>
+  </si>
+  <si>
+    <t>groom_all_domains_the_same</t>
+  </si>
+  <si>
     <t>value_1</t>
-  </si>
-  <si>
-    <t>alignment_enabled</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>alignment_method</t>
-  </si>
-  <si>
-    <t>Center</t>
-  </si>
-  <si>
-    <t>antialias</t>
-  </si>
-  <si>
-    <t>pad</t>
-  </si>
-  <si>
-    <t>pad_value</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>fastmarching</t>
-  </si>
-  <si>
-    <t>blur</t>
-  </si>
-  <si>
-    <t>blur_sigma</t>
-  </si>
-  <si>
-    <t>2.000000</t>
-  </si>
-  <si>
-    <t>isolate</t>
-  </si>
-  <si>
-    <t>fill_holes</t>
-  </si>
-  <si>
-    <t>fill_mesh_holes</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>antialias_amount</t>
-  </si>
-  <si>
-    <t>groom_output_prefix</t>
-  </si>
-  <si>
-    <t>groomed1</t>
-  </si>
-  <si>
-    <t>convert_to_mesh</t>
-  </si>
-  <si>
-    <t>mesh_smooth</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_method</t>
-  </si>
-  <si>
-    <t>Laplacian</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_laplacian_iterations</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
-  </si>
-  <si>
-    <t>1.000000</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
-  </si>
-  <si>
-    <t>0.050000</t>
-  </si>
-  <si>
-    <t>crop</t>
-  </si>
-  <si>
-    <t>reflect</t>
-  </si>
-  <si>
-    <t>reflect_column</t>
-  </si>
-  <si>
-    <t>reflect_choice</t>
-  </si>
-  <si>
-    <t>reflect_axis</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>resample</t>
-  </si>
-  <si>
-    <t>isotropic</t>
-  </si>
-  <si>
-    <t>iso_spacing</t>
-  </si>
-  <si>
-    <t>spacing</t>
-  </si>
-  <si>
-    <t>1 1 1</t>
-  </si>
-  <si>
-    <t>remesh</t>
-  </si>
-  <si>
-    <t>remesh_percent_mode</t>
-  </si>
-  <si>
-    <t>remesh_percent</t>
-  </si>
-  <si>
-    <t>75.000000</t>
-  </si>
-  <si>
-    <t>remesh_num_vertices</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>remesh_gradation</t>
-  </si>
-  <si>
-    <t>groom_all_domains_the_same</t>
   </si>
   <si>
     <t>number_of_particles</t>
@@ -1674,7 +1677,7 @@
     <t>tool_state</t>
   </si>
   <si>
-    <t>groom</t>
+    <t>optimize</t>
   </si>
   <si>
     <t>version</t>
@@ -3780,7 +3783,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3791,188 +3794,257 @@
         <v>458</v>
       </c>
       <c r="C1" t="s">
-        <v>459</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" t="s">
         <v>460</v>
       </c>
       <c r="C2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" t="s">
         <v>462</v>
       </c>
       <c r="C3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>464</v>
+        <v>463</v>
+      </c>
+      <c r="B4" t="s">
+        <v>460</v>
       </c>
       <c r="C4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>465</v>
+        <v>464</v>
+      </c>
+      <c r="B5" t="s">
+        <v>460</v>
       </c>
       <c r="C5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6" t="s">
         <v>466</v>
       </c>
       <c r="C6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>468</v>
+        <v>467</v>
+      </c>
+      <c r="B7" t="s">
+        <v>460</v>
       </c>
       <c r="C7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>469</v>
+        <v>468</v>
+      </c>
+      <c r="B8" t="s">
+        <v>460</v>
       </c>
       <c r="C8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>469</v>
+      </c>
+      <c r="B9" t="s">
         <v>470</v>
       </c>
       <c r="C9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>472</v>
+        <v>471</v>
+      </c>
+      <c r="B10" t="s">
+        <v>460</v>
       </c>
       <c r="C10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>472</v>
+      </c>
+      <c r="B11" t="s">
+        <v>460</v>
       </c>
       <c r="C11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>473</v>
+      </c>
+      <c r="B12" t="s">
         <v>474</v>
       </c>
       <c r="C12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>476</v>
+        <v>475</v>
+      </c>
+      <c r="B13" t="s">
+        <v>466</v>
       </c>
       <c r="C13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B14" t="s">
         <v>477</v>
       </c>
       <c r="C14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>479</v>
+        <v>478</v>
+      </c>
+      <c r="B15" t="s">
+        <v>474</v>
       </c>
       <c r="C15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>480</v>
+        <v>479</v>
+      </c>
+      <c r="B16" t="s">
+        <v>474</v>
       </c>
       <c r="C16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B17" t="s">
         <v>481</v>
       </c>
       <c r="C17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>483</v>
+        <v>482</v>
+      </c>
+      <c r="B18" t="s">
+        <v>466</v>
       </c>
       <c r="C18" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>483</v>
+      </c>
+      <c r="B19" t="s">
         <v>484</v>
       </c>
       <c r="C19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>486</v>
+        <v>485</v>
+      </c>
+      <c r="B20" t="s">
+        <v>466</v>
       </c>
       <c r="C20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>486</v>
+      </c>
+      <c r="B21" t="s">
         <v>487</v>
       </c>
       <c r="C21" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>489</v>
+        <v>488</v>
+      </c>
+      <c r="B22" t="s">
+        <v>460</v>
       </c>
       <c r="C22" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>490</v>
+        <v>489</v>
+      </c>
+      <c r="B23" t="s">
+        <v>474</v>
       </c>
       <c r="C23" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>491</v>
+        <v>490</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
@@ -3980,7 +4052,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>492</v>
+        <v>491</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -3988,90 +4063,134 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>492</v>
+      </c>
+      <c r="B26" t="s">
         <v>493</v>
       </c>
       <c r="C26" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>495</v>
+        <v>494</v>
+      </c>
+      <c r="B27" t="s">
+        <v>460</v>
       </c>
       <c r="C27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>496</v>
+        <v>495</v>
+      </c>
+      <c r="B28" t="s">
+        <v>460</v>
       </c>
       <c r="C28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>497</v>
+        <v>496</v>
+      </c>
+      <c r="B29" t="s">
+        <v>484</v>
       </c>
       <c r="C29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>497</v>
+      </c>
+      <c r="B30" t="s">
         <v>498</v>
       </c>
       <c r="C30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>500</v>
+        <v>499</v>
+      </c>
+      <c r="B31" t="s">
+        <v>460</v>
       </c>
       <c r="C31" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>501</v>
+        <v>500</v>
+      </c>
+      <c r="B32" t="s">
+        <v>460</v>
       </c>
       <c r="C32" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>501</v>
+      </c>
+      <c r="B33" t="s">
         <v>502</v>
       </c>
       <c r="C33" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>503</v>
+      </c>
+      <c r="B34" t="s">
         <v>504</v>
       </c>
       <c r="C34" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>506</v>
+        <v>505</v>
+      </c>
+      <c r="B35" t="s">
+        <v>484</v>
       </c>
       <c r="C35" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>506</v>
+      </c>
+      <c r="B36" t="s">
+        <v>474</v>
+      </c>
+      <c r="C36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>507</v>
       </c>
-      <c r="C36" t="s">
-        <v>461</v>
+      <c r="B37" t="s">
+        <v>460</v>
+      </c>
+      <c r="C37" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -4093,162 +4212,162 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B3" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B6" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B7" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B8" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B10" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B11" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B17" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B19" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B20" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B21" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -4270,50 +4389,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B4" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B5" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B6" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B7" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -4335,10 +4454,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -4360,26 +4479,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B4" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -4401,106 +4520,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" t="s">
         <v>560</v>
-      </c>
-      <c r="B3" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B5" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B6" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B7" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B8" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B9" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B12" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B13" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B14" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -4514,19 +4633,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>